<commit_message>
prepare to fix inefficient
Signed-off-by: ibicdlcod <504161487@qq.com>
</commit_message>
<xml_diff>
--- a/doc/Mechanics.xlsx
+++ b/doc/Mechanics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\old\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GuoMuoRuoProject\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B265008-35C4-48A5-AB50-57E7F824A6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D1ED76-919B-4736-930F-029D0E518B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3157" yWindow="1290" windowWidth="15826" windowHeight="11333" xr2:uid="{179AA141-B4E0-45BD-BB0D-72F4C1F29321}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{179AA141-B4E0-45BD-BB0D-72F4C1F29321}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -716,12 +716,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -738,7 +744,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -746,6 +752,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1065,8 +1077,8 @@
   <dimension ref="A1:D94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B75" sqref="B75"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C87" sqref="C87:C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1097,7 +1109,7 @@
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1509,10 +1521,10 @@
       <c r="A44" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -1521,8 +1533,8 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="1" t="s">
+      <c r="B45" s="4"/>
+      <c r="C45" s="3" t="s">
         <v>87</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -1534,7 +1546,7 @@
       <c r="B46" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="3" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1564,7 +1576,7 @@
       <c r="B49" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" s="3" t="s">
         <v>102</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -1862,7 +1874,7 @@
       <c r="B78" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" s="3" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2007,30 +2019,14 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="D80:D82"/>
-    <mergeCell ref="C87:C91"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="A58:A94"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="A50:A54"/>
-    <mergeCell ref="A44:A49"/>
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B35:C35"/>
@@ -2043,14 +2039,30 @@
     <mergeCell ref="A18:A40"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="A50:A54"/>
+    <mergeCell ref="A44:A49"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="D80:D82"/>
+    <mergeCell ref="C87:C91"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="A58:A94"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B84:C84"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>